<commit_message>
Created a basic form and linked the HTML to CSS
</commit_message>
<xml_diff>
--- a/RTS_TimePlan.xlsx
+++ b/RTS_TimePlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vineeth/Documents/HIS/Semester 2/RTS/SchedulingSimulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjathin/Documents/GitHub/SchedulingSimulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5D9E30-071F-6E43-866C-21656E53E4C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06F08B2-C4B0-7347-B185-669A02BF3BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1B2820E4-A953-CF4B-A245-983D6BC91716}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16980" xr2:uid="{1B2820E4-A953-CF4B-A245-983D6BC91716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t xml:space="preserve">Project Name: </t>
   </si>
@@ -60,9 +60,6 @@
     <t>Project Initiation and Planning</t>
   </si>
   <si>
-    <t>Process Plan</t>
-  </si>
-  <si>
     <t>Scheduling Algorithms</t>
   </si>
   <si>
@@ -111,7 +108,31 @@
     <t>Design</t>
   </si>
   <si>
-    <t>7 days</t>
+    <t>6 days</t>
+  </si>
+  <si>
+    <t>5 days</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>10 days</t>
+  </si>
+  <si>
+    <t>25 days</t>
+  </si>
+  <si>
+    <t>12 days</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>4 days</t>
   </si>
 </sst>
 </file>
@@ -119,7 +140,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -223,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -237,6 +258,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,9 +278,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,43 +593,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431C192D-A722-734E-B27C-1B88CE15707F}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -624,196 +653,249 @@
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="6">
         <v>43963</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="6">
+        <v>43963</v>
+      </c>
+      <c r="F3" s="6">
+        <v>43969</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6">
+        <v>43966</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="9">
-        <v>43963</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E4" s="6">
+        <v>43966</v>
+      </c>
+      <c r="F4" s="6">
+        <v>43969</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6">
+        <v>43967</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="6">
+        <v>43967</v>
+      </c>
+      <c r="F5" s="6">
+        <v>43969</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6">
         <v>43970</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="D6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="6">
+        <v>43970</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6">
+        <v>43969</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="6">
+        <v>43969</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43972</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6">
+        <v>43983</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6">
+        <v>43970</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6">
+        <v>43983</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6">
+        <v>43994</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6">
+        <v>44005</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A4:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>